<commit_message>
everyhing works correctly and peeerfectly
</commit_message>
<xml_diff>
--- a/pract2/Charts.xlsx
+++ b/pract2/Charts.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Листик" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -31,94 +31,25 @@
     <t xml:space="preserve">с использованием mpi</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">Ускорение</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">: Sp = T1 / Tp, где T1 - время работы </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">ПОСЛЕДОВАТЕЛЬНОЙ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> программы. Tp - время работы параллельной программы на p процессах/потоках.</t>
-    </r>
+    <t xml:space="preserve">Ускорение: Sp = T1 / Tp, где T1 - время работы ПОСЛЕДОВАТЕЛЬНОЙ программы. Tp - время работы параллельной программы на p процессах/потоках.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">Эффективность</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">: Ep = Sp / p * 100%</t>
-    </r>
+    <t xml:space="preserve"> Эффективность: Ep = Sp / p * 100%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="0.00000%"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
+    <numFmt numFmtId="169" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -149,14 +80,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -231,7 +154,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,28 +171,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -299,8 +206,8 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF5B9BD5"/>
-      <rgbColor rgb="FF7030A0"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
@@ -326,11 +233,11 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFC000"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF595959"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF70AD47"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -370,7 +277,7 @@
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Зависимость от времени</a:t>
+              <a:t>Зависисмость по времени</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -393,7 +300,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$B$1</c:f>
+              <c:f>Листик!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -404,17 +311,23 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ffff00"/>
+              <a:srgbClr val="ffc000"/>
             </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="ffff00"/>
+                <a:srgbClr val="ffc000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffc000"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:txPr>
@@ -442,25 +355,22 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$A$2:$A$7</c:f>
+              <c:f>Листик!$A$2:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>24</c:v>
                 </c:pt>
               </c:strCache>
@@ -468,27 +378,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$2:$B$7</c:f>
+              <c:f>Листик!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>51.0064</c:v>
+                  <c:v>53.0077</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.0064</c:v>
+                  <c:v>53.0077</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.0064</c:v>
+                  <c:v>53.0077</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.0064</c:v>
+                  <c:v>53.0077</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51.0064</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>51.0064</c:v>
+                  <c:v>53.0077</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -500,7 +407,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$C$1</c:f>
+              <c:f>Листик!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -511,17 +418,23 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="7030a0"/>
+              <a:srgbClr val="70ad47"/>
             </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="7030a0"/>
+                <a:srgbClr val="70ad47"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="70ad47"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:txPr>
@@ -549,25 +462,22 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$A$2:$A$7</c:f>
+              <c:f>Листик!$A$2:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>24</c:v>
                 </c:pt>
               </c:strCache>
@@ -575,27 +485,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$C$2:$C$7</c:f>
+              <c:f>Листик!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6.26128</c:v>
+                  <c:v>29.2698</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.98342</c:v>
+                  <c:v>21.1732</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.16029</c:v>
+                  <c:v>23.2108</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.84773</c:v>
+                  <c:v>4.08491</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99935</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.57067</c:v>
+                  <c:v>2.96406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -609,12 +516,12 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="37121816"/>
-        <c:axId val="71443159"/>
+        <c:marker val="1"/>
+        <c:axId val="31838681"/>
+        <c:axId val="3679217"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37121816"/>
+        <c:axId val="31838681"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,14 +553,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.387856328392246"/>
-              <c:y val="0.818590869183494"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -688,7 +587,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71443159"/>
+        <c:crossAx val="3679217"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -696,7 +595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71443159"/>
+        <c:axId val="3679217"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -733,7 +632,7 @@
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
-                  <a:t>Время, сек</a:t>
+                  <a:t>Время работы, сек</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -747,15 +646,12 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
-        <c:majorTickMark val="in"/>
-        <c:minorTickMark val="in"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:round/>
+            <a:noFill/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -772,7 +668,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37121816"/>
+        <c:crossAx val="31838681"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -785,16 +681,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.302306352330959"/>
-          <c:y val="0.879180014295347"/>
-          <c:w val="0.697693647669041"/>
-          <c:h val="0.0653314677128774"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -883,7 +769,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$B$23</c:f>
+              <c:f>"с использованием mpi"</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -894,17 +780,23 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="7030a0"/>
+              <a:srgbClr val="ffc000"/>
             </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="7030a0"/>
+                <a:srgbClr val="ffc000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffc000"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:txPr>
@@ -932,9 +824,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$A$24:$A$29</c:f>
+              <c:f>Листик!$A$20:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -949,33 +841,30 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$24:$B$29</c:f>
+              <c:f>Листик!$B$20:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8.14632151892265</c:v>
+                  <c:v>1.81100315000444</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.0966206568301</c:v>
+                  <c:v>2.50352804488693</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.6109040915803</c:v>
+                  <c:v>2.28375152946042</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.6048989841589</c:v>
+                  <c:v>12.9764670457856</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51.0395757242207</c:v>
+                  <c:v>17.8834773924954</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -989,12 +878,12 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="41917747"/>
-        <c:axId val="28591585"/>
+        <c:marker val="1"/>
+        <c:axId val="93181145"/>
+        <c:axId val="26979913"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41917747"/>
+        <c:axId val="93181145"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1060,7 +949,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28591585"/>
+        <c:crossAx val="26979913"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1068,7 +957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28591585"/>
+        <c:axId val="26979913"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,7 +996,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41917747"/>
+        <c:crossAx val="93181145"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1208,7 +1097,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$B$39:$B$39</c:f>
+              <c:f>Листик!$B$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1219,17 +1108,23 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="7030a0"/>
+              <a:srgbClr val="ffc000"/>
             </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="7030a0"/>
+                <a:srgbClr val="ffc000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffc000"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:txPr>
@@ -1257,7 +1152,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$A$40:$A$44</c:f>
+              <c:f>Листик!$A$36:$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1280,24 +1175,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$40:$B$44</c:f>
+              <c:f>Листик!$B$36:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>407.316075946132</c:v>
+                  <c:v>0.905501575002221</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>427.415516420752</c:v>
+                  <c:v>0.625882011221733</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>295.136301144754</c:v>
+                  <c:v>0.285468941182553</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>172.530618650993</c:v>
+                  <c:v>0.811029190361599</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>212.66489885092</c:v>
+                  <c:v>0.745144891353976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1311,12 +1206,12 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="66619269"/>
-        <c:axId val="17771812"/>
+        <c:marker val="1"/>
+        <c:axId val="6475974"/>
+        <c:axId val="60677473"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66619269"/>
+        <c:axId val="6475974"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1382,7 +1277,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17771812"/>
+        <c:crossAx val="60677473"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1390,7 +1285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17771812"/>
+        <c:axId val="60677473"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,7 +1301,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1429,7 +1324,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66619269"/>
+        <c:crossAx val="6475974"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1486,24 +1381,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>76680</xdr:colOff>
+      <xdr:colOff>68760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>201960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>319680</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>373320</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Диаграмма 1"/>
+        <xdr:cNvPr id="0" name="Диаграмма 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5673960" y="95400"/>
-        <a:ext cx="6313680" cy="3280320"/>
+        <a:off x="5409000" y="201960"/>
+        <a:ext cx="5616360" cy="2567520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1515,25 +1410,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>441000</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>117720</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>122040</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>26640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>308160</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>426600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Диаграмма 2"/>
+        <xdr:cNvPr id="1" name="Диаграмма 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5279400" y="4232520"/>
-        <a:ext cx="7455600" cy="3756240"/>
+        <a:off x="6221160" y="3737520"/>
+        <a:ext cx="5616360" cy="2575080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1546,24 +1441,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>78120</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:colOff>354240</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>587880</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>48960</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>105840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 3"/>
+        <xdr:cNvPr id="2" name="Диаграмма 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4916520" y="8731080"/>
-        <a:ext cx="7339320" cy="3790800"/>
+        <a:off x="4935600" y="6663600"/>
+        <a:ext cx="5765400" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1581,20 +1476,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W69" activeCellId="0" sqref="W69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.44"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1607,229 +1502,175 @@
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>51.0064</v>
+        <v>53.0077</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>6.26128</v>
+        <v>29.2698</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>51.0064</v>
+        <v>53.0077</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>2.98342</v>
+        <v>21.1732</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>51.0064</v>
+        <v>53.0077</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>2.16029</v>
+        <v>23.2108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>51.0064</v>
+        <v>53.0077</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>1.84773</v>
+        <v>4.08491</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>53.0077</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>2.96406</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <f aca="false">B2/C2</f>
+        <v>1.81100315000444</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <f aca="false">B3/C3</f>
+        <v>2.50352804488693</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <f aca="false">B4/C4</f>
+        <v>2.28375152946042</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>51.0064</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>0.99935</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="B23" s="3" t="n">
+        <f aca="false">B5/C5</f>
+        <v>12.9764670457856</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="B7" s="3" t="n">
-        <v>51.0064</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>0.57067</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="B24" s="3" t="n">
+        <f aca="false">B6/C6</f>
+        <v>17.8834773924954</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
+    <row r="36" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B24" s="3" t="n">
-        <f aca="false">B2/C2</f>
-        <v>8.14632151892265</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="n">
+      <c r="B36" s="5" t="n">
+        <f aca="false">B20/A36</f>
+        <v>0.905501575002221</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B25" s="3" t="n">
-        <f aca="false">B3/C3</f>
-        <v>17.0966206568301</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="n">
+      <c r="B37" s="5" t="n">
+        <f aca="false">B21/A37</f>
+        <v>0.625882011221733</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B26" s="3" t="n">
-        <f aca="false">B4/C4</f>
-        <v>23.6109040915803</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+      <c r="B38" s="5" t="n">
+        <f aca="false">B22/A38</f>
+        <v>0.285468941182553</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="B27" s="3" t="n">
-        <f aca="false">B5/C5</f>
-        <v>27.6048989841589</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
+      <c r="B39" s="5" t="n">
+        <f aca="false">B23/A39</f>
+        <v>0.811029190361599</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="B28" s="3" t="n">
-        <f aca="false">B6/C6</f>
-        <v>51.0395757242207</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B40" s="3" t="n">
-        <f aca="false">B24/A40*100</f>
-        <v>407.316075946132</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B41" s="3" t="n">
-        <f aca="false">B25/A41*100</f>
-        <v>427.415516420752</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B42" s="3" t="n">
-        <f aca="false">B26/A42*100</f>
-        <v>295.136301144754</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="B43" s="3" t="n">
-        <f aca="false">B27/A43*100</f>
-        <v>172.530618650993</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="B44" s="3" t="n">
-        <f aca="false">B28/A44*100</f>
-        <v>212.66489885092</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="9"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B40" s="5" t="n">
+        <f aca="false">B24/A40</f>
+        <v>0.745144891353976</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>